<commit_message>
aggiornamento data.json (malformato) e report.checklist.xlsx (aggiornato caso 40)
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GASNETGROUPXX/gasnet/SaniPocket/V1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GASNETGROUPXX/gasnet/SaniPocket/V1.0/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gasnetit.sharepoint.com/sites/softwarehouse/Shared Documents/Ticket SWH/#132841 - Gas.Net Group - Simone Bettini - Supplemento analisi specifiche XDS vs Documentale/20240610_richiesta_accreditamento/A1#111#GASNETGROUPXX/gasnet/SaniPocket/V1.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE-GTW\GitHubRepo\it-fse-accreditamento\GATEWAY\A1#111#GASNETGROUPXX\gasnet\SaniPocket\V1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{810550F0-DD46-4570-80D4-621F663A4072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14960DAE-AAF3-4941-A03A-4E69ECB68EAD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B94AB5B-B5CD-4224-8047-C8239DE30D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4015,12 +4015,6 @@
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>2024-06-10T08:06:59Z</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nelle colonne relative a:
 "ERRORE BLOCCANTE (SI/NO)", "ERRORE VISIBILE A UTENTE (SI/NO)", "MESSAGGIO DI ERRORE", "GESTITO IN BACKOFFICE (SI/NO)", "GESTIONE ERRORE".</t>
   </si>
@@ -4272,6 +4266,12 @@
   </si>
   <si>
     <t>Monitoraggio CheckMk - Operatore di Backoffice - Reinvio manuale - Il medico può proseguire a produrre il documento</t>
+  </si>
+  <si>
+    <t>2024-07-16T07:40:13Z</t>
+  </si>
+  <si>
+    <t>ee6a5105e2b627dd</t>
   </si>
 </sst>
 </file>
@@ -4281,7 +4281,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4406,6 +4406,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -4805,7 +4812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4995,36 +5002,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6504,10 +6483,10 @@
   <dimension ref="A1:W968"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="AA173" sqref="AA173"/>
+      <selection pane="bottomRight" activeCell="I392" sqref="I391:I392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6517,7 +6496,8 @@
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="4" width="63.85546875" customWidth="1"/>
     <col min="5" max="5" width="104.85546875" customWidth="1"/>
-    <col min="6" max="9" width="33.140625" customWidth="1"/>
+    <col min="6" max="8" width="33.140625" customWidth="1"/>
+    <col min="9" max="9" width="147.28515625" customWidth="1"/>
     <col min="10" max="10" width="27.140625" customWidth="1"/>
     <col min="11" max="18" width="36.42578125" customWidth="1"/>
     <col min="19" max="19" width="55.140625" customWidth="1"/>
@@ -7864,62 +7844,62 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:23" s="80" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="73">
+    <row r="39" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="31">
         <v>32</v>
       </c>
-      <c r="B39" s="74" t="s">
+      <c r="B39" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="74" t="s">
+      <c r="C39" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D39" s="74" t="s">
+      <c r="D39" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="75" t="s">
+      <c r="E39" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F39" s="76">
+      <c r="F39" s="19">
         <v>45453</v>
       </c>
-      <c r="G39" s="77" t="s">
+      <c r="G39" s="60" t="s">
         <v>840</v>
       </c>
-      <c r="H39" s="78" t="s">
+      <c r="H39" s="20" t="s">
         <v>841</v>
       </c>
-      <c r="I39" s="78" t="s">
+      <c r="I39" s="20" t="s">
         <v>842</v>
       </c>
-      <c r="J39" s="79" t="s">
+      <c r="J39" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K39" s="79"/>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79" t="s">
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21" t="s">
         <v>780</v>
       </c>
-      <c r="N39" s="79" t="s">
+      <c r="N39" s="21" t="s">
         <v>780</v>
       </c>
       <c r="O39" s="21"/>
-      <c r="P39" s="79" t="s">
+      <c r="P39" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="Q39" s="79" t="s">
+      <c r="Q39" s="21" t="s">
         <v>780</v>
       </c>
-      <c r="R39" s="79" t="s">
+      <c r="R39" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="S39" s="79" t="s">
-        <v>923</v>
-      </c>
-      <c r="T39" s="79"/>
-      <c r="U39" s="79"/>
-      <c r="V39" s="79"/>
-      <c r="W39" s="81" t="s">
+      <c r="S39" s="21" t="s">
+        <v>921</v>
+      </c>
+      <c r="T39" s="21"/>
+      <c r="U39" s="21"/>
+      <c r="V39" s="21"/>
+      <c r="W39" s="24" t="s">
         <v>73</v>
       </c>
     </row>
@@ -8182,62 +8162,62 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:23" s="80" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="73">
+    <row r="47" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="31">
         <v>40</v>
       </c>
-      <c r="B47" s="74" t="s">
+      <c r="B47" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="74" t="s">
+      <c r="C47" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D47" s="74" t="s">
+      <c r="D47" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E47" s="75" t="s">
+      <c r="E47" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="F47" s="76">
-        <v>45453</v>
-      </c>
-      <c r="G47" s="77" t="s">
-        <v>843</v>
-      </c>
-      <c r="H47" s="78" t="s">
-        <v>844</v>
-      </c>
-      <c r="I47" s="78" t="s">
-        <v>844</v>
-      </c>
-      <c r="J47" s="79" t="s">
+      <c r="F47" s="19">
+        <v>45489</v>
+      </c>
+      <c r="G47" s="60" t="s">
+        <v>922</v>
+      </c>
+      <c r="H47" s="20" t="s">
+        <v>923</v>
+      </c>
+      <c r="I47" s="20" t="s">
+        <v>842</v>
+      </c>
+      <c r="J47" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K47" s="79"/>
-      <c r="L47" s="79"/>
-      <c r="M47" s="79" t="s">
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21" t="s">
         <v>780</v>
       </c>
-      <c r="N47" s="79" t="s">
+      <c r="N47" s="21" t="s">
         <v>780</v>
       </c>
       <c r="O47" s="21"/>
-      <c r="P47" s="79" t="s">
+      <c r="P47" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="Q47" s="79" t="s">
+      <c r="Q47" s="21" t="s">
         <v>780</v>
       </c>
-      <c r="R47" s="79" t="s">
+      <c r="R47" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="S47" s="79" t="s">
-        <v>923</v>
-      </c>
-      <c r="T47" s="79"/>
-      <c r="U47" s="79"/>
-      <c r="V47" s="79"/>
-      <c r="W47" s="81" t="s">
+      <c r="S47" s="21" t="s">
+        <v>921</v>
+      </c>
+      <c r="T47" s="21"/>
+      <c r="U47" s="21"/>
+      <c r="V47" s="21"/>
+      <c r="W47" s="24" t="s">
         <v>73</v>
       </c>
     </row>
@@ -8508,56 +8488,56 @@
         <v>73</v>
       </c>
     </row>
-    <row r="55" spans="1:23" s="80" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="73">
+    <row r="55" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="31">
         <v>48</v>
       </c>
-      <c r="B55" s="74" t="s">
+      <c r="B55" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C55" s="74" t="s">
+      <c r="C55" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="74" t="s">
+      <c r="D55" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="E55" s="75" t="s">
-        <v>845</v>
-      </c>
-      <c r="F55" s="76"/>
-      <c r="G55" s="77"/>
-      <c r="H55" s="78"/>
-      <c r="I55" s="78"/>
-      <c r="J55" s="79" t="s">
+      <c r="E55" s="18" t="s">
+        <v>843</v>
+      </c>
+      <c r="F55" s="19"/>
+      <c r="G55" s="60"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K55" s="79"/>
-      <c r="L55" s="79"/>
-      <c r="M55" s="79" t="s">
+      <c r="K55" s="21"/>
+      <c r="L55" s="21"/>
+      <c r="M55" s="21" t="s">
         <v>780</v>
       </c>
-      <c r="N55" s="79" t="s">
+      <c r="N55" s="21" t="s">
         <v>780</v>
       </c>
       <c r="O55" s="21"/>
-      <c r="P55" s="79" t="s">
+      <c r="P55" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="Q55" s="79" t="s">
+      <c r="Q55" s="21" t="s">
         <v>780</v>
       </c>
-      <c r="R55" s="79" t="s">
+      <c r="R55" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="S55" s="79" t="s">
-        <v>923</v>
-      </c>
-      <c r="T55" s="79"/>
-      <c r="U55" s="82" t="s">
+      <c r="S55" s="21" t="s">
+        <v>921</v>
+      </c>
+      <c r="T55" s="21"/>
+      <c r="U55" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="V55" s="79"/>
-      <c r="W55" s="81" t="s">
+      <c r="V55" s="21"/>
+      <c r="W55" s="24" t="s">
         <v>73</v>
       </c>
     </row>
@@ -12193,309 +12173,309 @@
         <v>73</v>
       </c>
     </row>
-    <row r="154" spans="1:23" s="80" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="73">
+    <row r="154" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A154" s="31">
         <v>147</v>
       </c>
-      <c r="B154" s="74" t="s">
+      <c r="B154" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C154" s="74" t="s">
+      <c r="C154" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D154" s="74" t="s">
+      <c r="D154" s="17" t="s">
         <v>291</v>
       </c>
-      <c r="E154" s="75" t="s">
+      <c r="E154" s="18" t="s">
+        <v>844</v>
+      </c>
+      <c r="F154" s="19">
+        <v>45453</v>
+      </c>
+      <c r="G154" s="60" t="s">
+        <v>845</v>
+      </c>
+      <c r="H154" s="20" t="s">
         <v>846</v>
       </c>
-      <c r="F154" s="76">
+      <c r="I154" s="20" t="s">
+        <v>847</v>
+      </c>
+      <c r="J154" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="K154" s="21"/>
+      <c r="L154" s="21"/>
+      <c r="M154" s="21"/>
+      <c r="N154" s="21"/>
+      <c r="O154" s="21"/>
+      <c r="P154" s="21"/>
+      <c r="Q154" s="21"/>
+      <c r="R154" s="21"/>
+      <c r="S154" s="21"/>
+      <c r="T154" s="21"/>
+      <c r="U154" s="22"/>
+      <c r="V154" s="21"/>
+      <c r="W154" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="155" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A155" s="31">
+        <v>148</v>
+      </c>
+      <c r="B155" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C155" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D155" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="E155" s="18" t="s">
+        <v>848</v>
+      </c>
+      <c r="F155" s="19">
         <v>45453</v>
       </c>
-      <c r="G154" s="77" t="s">
-        <v>847</v>
-      </c>
-      <c r="H154" s="78" t="s">
-        <v>848</v>
-      </c>
-      <c r="I154" s="78" t="s">
+      <c r="G155" s="60" t="s">
         <v>849</v>
       </c>
-      <c r="J154" s="79" t="s">
+      <c r="H155" s="20" t="s">
+        <v>850</v>
+      </c>
+      <c r="I155" s="20" t="s">
+        <v>851</v>
+      </c>
+      <c r="J155" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K154" s="79"/>
-      <c r="L154" s="79"/>
-      <c r="M154" s="79"/>
-      <c r="N154" s="79"/>
-      <c r="O154" s="21"/>
-      <c r="P154" s="79"/>
-      <c r="Q154" s="79"/>
-      <c r="R154" s="79"/>
-      <c r="S154" s="79"/>
-      <c r="T154" s="79"/>
-      <c r="U154" s="82"/>
-      <c r="V154" s="79"/>
-      <c r="W154" s="81" t="s">
+      <c r="K155" s="21"/>
+      <c r="L155" s="21"/>
+      <c r="M155" s="21"/>
+      <c r="N155" s="21"/>
+      <c r="O155" s="21"/>
+      <c r="P155" s="21"/>
+      <c r="Q155" s="21"/>
+      <c r="R155" s="21"/>
+      <c r="S155" s="21"/>
+      <c r="T155" s="21"/>
+      <c r="U155" s="22"/>
+      <c r="V155" s="21"/>
+      <c r="W155" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="155" spans="1:23" s="80" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="73">
-        <v>148</v>
-      </c>
-      <c r="B155" s="74" t="s">
+    <row r="156" spans="1:23" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A156" s="31">
+        <v>149</v>
+      </c>
+      <c r="B156" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C155" s="74" t="s">
+      <c r="C156" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D155" s="74" t="s">
-        <v>292</v>
-      </c>
-      <c r="E155" s="75" t="s">
-        <v>850</v>
-      </c>
-      <c r="F155" s="76">
+      <c r="D156" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="E156" s="18" t="s">
+        <v>852</v>
+      </c>
+      <c r="F156" s="19">
         <v>45453</v>
       </c>
-      <c r="G155" s="77" t="s">
-        <v>851</v>
-      </c>
-      <c r="H155" s="78" t="s">
-        <v>852</v>
-      </c>
-      <c r="I155" s="78" t="s">
+      <c r="G156" s="60" t="s">
         <v>853</v>
       </c>
-      <c r="J155" s="79" t="s">
+      <c r="H156" s="20" t="s">
+        <v>854</v>
+      </c>
+      <c r="I156" s="20" t="s">
+        <v>855</v>
+      </c>
+      <c r="J156" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K155" s="79"/>
-      <c r="L155" s="79"/>
-      <c r="M155" s="79"/>
-      <c r="N155" s="79"/>
-      <c r="O155" s="21"/>
-      <c r="P155" s="79"/>
-      <c r="Q155" s="79"/>
-      <c r="R155" s="79"/>
-      <c r="S155" s="79"/>
-      <c r="T155" s="79"/>
-      <c r="U155" s="82"/>
-      <c r="V155" s="79"/>
-      <c r="W155" s="81" t="s">
+      <c r="K156" s="21"/>
+      <c r="L156" s="21"/>
+      <c r="M156" s="21"/>
+      <c r="N156" s="21"/>
+      <c r="O156" s="21"/>
+      <c r="P156" s="21"/>
+      <c r="Q156" s="21"/>
+      <c r="R156" s="21"/>
+      <c r="S156" s="21"/>
+      <c r="T156" s="21"/>
+      <c r="U156" s="22"/>
+      <c r="V156" s="23"/>
+      <c r="W156" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="156" spans="1:23" s="80" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="73">
-        <v>149</v>
-      </c>
-      <c r="B156" s="74" t="s">
+    <row r="157" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="31">
+        <v>150</v>
+      </c>
+      <c r="B157" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C156" s="74" t="s">
+      <c r="C157" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D156" s="74" t="s">
-        <v>293</v>
-      </c>
-      <c r="E156" s="75" t="s">
-        <v>854</v>
-      </c>
-      <c r="F156" s="76">
+      <c r="D157" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="E157" s="18" t="s">
+        <v>856</v>
+      </c>
+      <c r="F157" s="19">
         <v>45453</v>
       </c>
-      <c r="G156" s="77" t="s">
-        <v>855</v>
-      </c>
-      <c r="H156" s="78" t="s">
-        <v>856</v>
-      </c>
-      <c r="I156" s="78" t="s">
+      <c r="G157" s="60" t="s">
         <v>857</v>
       </c>
-      <c r="J156" s="79" t="s">
+      <c r="H157" s="20" t="s">
+        <v>858</v>
+      </c>
+      <c r="I157" s="20" t="s">
+        <v>859</v>
+      </c>
+      <c r="J157" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K156" s="79"/>
-      <c r="L156" s="79"/>
-      <c r="M156" s="79"/>
-      <c r="N156" s="79"/>
-      <c r="O156" s="21"/>
-      <c r="P156" s="79"/>
-      <c r="Q156" s="79"/>
-      <c r="R156" s="79"/>
-      <c r="S156" s="79"/>
-      <c r="T156" s="79"/>
-      <c r="U156" s="82"/>
-      <c r="V156" s="83"/>
-      <c r="W156" s="81" t="s">
+      <c r="K157" s="21"/>
+      <c r="L157" s="21"/>
+      <c r="M157" s="21"/>
+      <c r="N157" s="21"/>
+      <c r="O157" s="21"/>
+      <c r="P157" s="21"/>
+      <c r="Q157" s="21"/>
+      <c r="R157" s="21"/>
+      <c r="S157" s="21"/>
+      <c r="T157" s="21"/>
+      <c r="U157" s="22"/>
+      <c r="V157" s="23"/>
+      <c r="W157" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="157" spans="1:23" s="80" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="73">
-        <v>150</v>
-      </c>
-      <c r="B157" s="74" t="s">
+    <row r="158" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A158" s="31">
+        <v>151</v>
+      </c>
+      <c r="B158" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C157" s="74" t="s">
+      <c r="C158" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D157" s="74" t="s">
-        <v>294</v>
-      </c>
-      <c r="E157" s="75" t="s">
-        <v>858</v>
-      </c>
-      <c r="F157" s="76">
+      <c r="D158" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="E158" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="F158" s="19">
         <v>45453</v>
       </c>
-      <c r="G157" s="77" t="s">
-        <v>859</v>
-      </c>
-      <c r="H157" s="78" t="s">
+      <c r="G158" s="60" t="s">
         <v>860</v>
       </c>
-      <c r="I157" s="78" t="s">
+      <c r="H158" s="20" t="s">
         <v>861</v>
       </c>
-      <c r="J157" s="79" t="s">
+      <c r="I158" s="20" t="s">
+        <v>862</v>
+      </c>
+      <c r="J158" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K157" s="79"/>
-      <c r="L157" s="79"/>
-      <c r="M157" s="79"/>
-      <c r="N157" s="79"/>
-      <c r="O157" s="21"/>
-      <c r="P157" s="79"/>
-      <c r="Q157" s="79"/>
-      <c r="R157" s="79"/>
-      <c r="S157" s="79"/>
-      <c r="T157" s="79"/>
-      <c r="U157" s="82"/>
-      <c r="V157" s="83"/>
-      <c r="W157" s="81" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="158" spans="1:23" s="80" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="73">
-        <v>151</v>
-      </c>
-      <c r="B158" s="74" t="s">
+      <c r="K158" s="21"/>
+      <c r="L158" s="21"/>
+      <c r="M158" s="21" t="s">
+        <v>780</v>
+      </c>
+      <c r="N158" s="21" t="s">
+        <v>780</v>
+      </c>
+      <c r="O158" s="21"/>
+      <c r="P158" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q158" s="21" t="s">
+        <v>780</v>
+      </c>
+      <c r="R158" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="S158" s="21" t="s">
+        <v>921</v>
+      </c>
+      <c r="T158" s="21"/>
+      <c r="U158" s="22"/>
+      <c r="V158" s="23"/>
+      <c r="W158" s="24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="159" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A159" s="31">
+        <v>152</v>
+      </c>
+      <c r="B159" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C158" s="74" t="s">
+      <c r="C159" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D158" s="74" t="s">
-        <v>295</v>
-      </c>
-      <c r="E158" s="75" t="s">
-        <v>296</v>
-      </c>
-      <c r="F158" s="76">
+      <c r="D159" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="E159" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="F159" s="19">
         <v>45453</v>
       </c>
-      <c r="G158" s="77" t="s">
-        <v>862</v>
-      </c>
-      <c r="H158" s="78" t="s">
+      <c r="G159" s="60" t="s">
         <v>863</v>
       </c>
-      <c r="I158" s="78" t="s">
+      <c r="H159" s="20" t="s">
         <v>864</v>
       </c>
-      <c r="J158" s="79" t="s">
+      <c r="I159" s="20" t="s">
+        <v>865</v>
+      </c>
+      <c r="J159" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K158" s="79"/>
-      <c r="L158" s="79"/>
-      <c r="M158" s="79" t="s">
+      <c r="K159" s="21"/>
+      <c r="L159" s="21"/>
+      <c r="M159" s="21" t="s">
         <v>780</v>
       </c>
-      <c r="N158" s="79" t="s">
+      <c r="N159" s="21" t="s">
         <v>780</v>
       </c>
-      <c r="O158" s="21"/>
-      <c r="P158" s="79" t="s">
+      <c r="O159" s="21"/>
+      <c r="P159" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="Q158" s="79" t="s">
+      <c r="Q159" s="21" t="s">
         <v>780</v>
       </c>
-      <c r="R158" s="79" t="s">
+      <c r="R159" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="S158" s="79" t="s">
-        <v>923</v>
-      </c>
-      <c r="T158" s="79"/>
-      <c r="U158" s="82"/>
-      <c r="V158" s="83"/>
-      <c r="W158" s="81" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="159" spans="1:23" s="80" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="73">
-        <v>152</v>
-      </c>
-      <c r="B159" s="74" t="s">
-        <v>38</v>
-      </c>
-      <c r="C159" s="74" t="s">
-        <v>78</v>
-      </c>
-      <c r="D159" s="74" t="s">
-        <v>297</v>
-      </c>
-      <c r="E159" s="75" t="s">
-        <v>298</v>
-      </c>
-      <c r="F159" s="76">
-        <v>45453</v>
-      </c>
-      <c r="G159" s="77" t="s">
-        <v>865</v>
-      </c>
-      <c r="H159" s="78" t="s">
-        <v>866</v>
-      </c>
-      <c r="I159" s="78" t="s">
-        <v>867</v>
-      </c>
-      <c r="J159" s="79" t="s">
-        <v>93</v>
-      </c>
-      <c r="K159" s="79"/>
-      <c r="L159" s="79"/>
-      <c r="M159" s="79" t="s">
-        <v>780</v>
-      </c>
-      <c r="N159" s="79" t="s">
-        <v>780</v>
-      </c>
-      <c r="O159" s="21"/>
-      <c r="P159" s="79" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q159" s="79" t="s">
-        <v>780</v>
-      </c>
-      <c r="R159" s="79" t="s">
-        <v>93</v>
-      </c>
-      <c r="S159" s="79" t="s">
-        <v>923</v>
-      </c>
-      <c r="T159" s="79"/>
-      <c r="U159" s="82"/>
-      <c r="V159" s="83"/>
-      <c r="W159" s="81" t="s">
+      <c r="S159" s="21" t="s">
+        <v>921</v>
+      </c>
+      <c r="T159" s="21"/>
+      <c r="U159" s="22"/>
+      <c r="V159" s="23"/>
+      <c r="W159" s="24" t="s">
         <v>73</v>
       </c>
     </row>
@@ -12519,13 +12499,13 @@
         <v>45453</v>
       </c>
       <c r="G160" s="60" t="s">
+        <v>866</v>
+      </c>
+      <c r="H160" s="20" t="s">
+        <v>867</v>
+      </c>
+      <c r="I160" s="20" t="s">
         <v>868</v>
-      </c>
-      <c r="H160" s="20" t="s">
-        <v>869</v>
-      </c>
-      <c r="I160" s="20" t="s">
-        <v>870</v>
       </c>
       <c r="J160" s="21" t="s">
         <v>93</v>
@@ -12549,7 +12529,7 @@
         <v>93</v>
       </c>
       <c r="S160" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T160" s="21"/>
       <c r="U160" s="22"/>
@@ -12578,13 +12558,13 @@
         <v>45453</v>
       </c>
       <c r="G161" s="60" t="s">
+        <v>869</v>
+      </c>
+      <c r="H161" s="20" t="s">
+        <v>870</v>
+      </c>
+      <c r="I161" s="20" t="s">
         <v>871</v>
-      </c>
-      <c r="H161" s="20" t="s">
-        <v>872</v>
-      </c>
-      <c r="I161" s="20" t="s">
-        <v>873</v>
       </c>
       <c r="J161" s="21" t="s">
         <v>93</v>
@@ -12608,7 +12588,7 @@
         <v>93</v>
       </c>
       <c r="S161" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T161" s="21"/>
       <c r="U161" s="22"/>
@@ -12637,13 +12617,13 @@
         <v>45453</v>
       </c>
       <c r="G162" s="60" t="s">
+        <v>872</v>
+      </c>
+      <c r="H162" s="20" t="s">
+        <v>873</v>
+      </c>
+      <c r="I162" s="20" t="s">
         <v>874</v>
-      </c>
-      <c r="H162" s="20" t="s">
-        <v>875</v>
-      </c>
-      <c r="I162" s="20" t="s">
-        <v>876</v>
       </c>
       <c r="J162" s="21" t="s">
         <v>93</v>
@@ -12667,7 +12647,7 @@
         <v>93</v>
       </c>
       <c r="S162" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T162" s="21"/>
       <c r="U162" s="22"/>
@@ -12696,13 +12676,13 @@
         <v>45453</v>
       </c>
       <c r="G163" s="60" t="s">
+        <v>875</v>
+      </c>
+      <c r="H163" s="20" t="s">
+        <v>876</v>
+      </c>
+      <c r="I163" s="20" t="s">
         <v>877</v>
-      </c>
-      <c r="H163" s="20" t="s">
-        <v>878</v>
-      </c>
-      <c r="I163" s="20" t="s">
-        <v>879</v>
       </c>
       <c r="J163" s="21" t="s">
         <v>93</v>
@@ -12726,7 +12706,7 @@
         <v>93</v>
       </c>
       <c r="S163" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T163" s="21"/>
       <c r="U163" s="22"/>
@@ -12755,13 +12735,13 @@
         <v>45453</v>
       </c>
       <c r="G164" s="60" t="s">
+        <v>878</v>
+      </c>
+      <c r="H164" s="20" t="s">
+        <v>879</v>
+      </c>
+      <c r="I164" s="20" t="s">
         <v>880</v>
-      </c>
-      <c r="H164" s="20" t="s">
-        <v>881</v>
-      </c>
-      <c r="I164" s="20" t="s">
-        <v>882</v>
       </c>
       <c r="J164" s="21" t="s">
         <v>93</v>
@@ -12785,7 +12765,7 @@
         <v>93</v>
       </c>
       <c r="S164" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T164" s="21"/>
       <c r="U164" s="22"/>
@@ -12814,13 +12794,13 @@
         <v>45453</v>
       </c>
       <c r="G165" s="60" t="s">
+        <v>881</v>
+      </c>
+      <c r="H165" s="20" t="s">
+        <v>882</v>
+      </c>
+      <c r="I165" s="20" t="s">
         <v>883</v>
-      </c>
-      <c r="H165" s="20" t="s">
-        <v>884</v>
-      </c>
-      <c r="I165" s="20" t="s">
-        <v>885</v>
       </c>
       <c r="J165" s="21" t="s">
         <v>93</v>
@@ -12844,7 +12824,7 @@
         <v>93</v>
       </c>
       <c r="S165" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T165" s="21"/>
       <c r="U165" s="22"/>
@@ -12873,13 +12853,13 @@
         <v>45453</v>
       </c>
       <c r="G166" s="60" t="s">
+        <v>884</v>
+      </c>
+      <c r="H166" s="20" t="s">
+        <v>885</v>
+      </c>
+      <c r="I166" s="20" t="s">
         <v>886</v>
-      </c>
-      <c r="H166" s="20" t="s">
-        <v>887</v>
-      </c>
-      <c r="I166" s="20" t="s">
-        <v>888</v>
       </c>
       <c r="J166" s="21" t="s">
         <v>93</v>
@@ -12903,7 +12883,7 @@
         <v>93</v>
       </c>
       <c r="S166" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T166" s="21"/>
       <c r="U166" s="22"/>
@@ -12932,13 +12912,13 @@
         <v>45453</v>
       </c>
       <c r="G167" s="60" t="s">
+        <v>887</v>
+      </c>
+      <c r="H167" s="20" t="s">
+        <v>888</v>
+      </c>
+      <c r="I167" s="20" t="s">
         <v>889</v>
-      </c>
-      <c r="H167" s="20" t="s">
-        <v>890</v>
-      </c>
-      <c r="I167" s="20" t="s">
-        <v>891</v>
       </c>
       <c r="J167" s="21" t="s">
         <v>93</v>
@@ -12962,7 +12942,7 @@
         <v>93</v>
       </c>
       <c r="S167" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T167" s="21"/>
       <c r="U167" s="22"/>
@@ -12991,13 +12971,13 @@
         <v>45453</v>
       </c>
       <c r="G168" s="60" t="s">
+        <v>890</v>
+      </c>
+      <c r="H168" s="20" t="s">
+        <v>891</v>
+      </c>
+      <c r="I168" s="20" t="s">
         <v>892</v>
-      </c>
-      <c r="H168" s="20" t="s">
-        <v>893</v>
-      </c>
-      <c r="I168" s="20" t="s">
-        <v>894</v>
       </c>
       <c r="J168" s="21" t="s">
         <v>93</v>
@@ -13021,7 +13001,7 @@
         <v>93</v>
       </c>
       <c r="S168" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T168" s="21"/>
       <c r="U168" s="22"/>
@@ -13050,13 +13030,13 @@
         <v>45453</v>
       </c>
       <c r="G169" s="60" t="s">
+        <v>893</v>
+      </c>
+      <c r="H169" s="20" t="s">
+        <v>894</v>
+      </c>
+      <c r="I169" s="20" t="s">
         <v>895</v>
-      </c>
-      <c r="H169" s="20" t="s">
-        <v>896</v>
-      </c>
-      <c r="I169" s="20" t="s">
-        <v>897</v>
       </c>
       <c r="J169" s="21" t="s">
         <v>93</v>
@@ -13080,7 +13060,7 @@
         <v>93</v>
       </c>
       <c r="S169" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T169" s="21"/>
       <c r="U169" s="22"/>
@@ -13109,13 +13089,13 @@
         <v>45453</v>
       </c>
       <c r="G170" s="60" t="s">
+        <v>896</v>
+      </c>
+      <c r="H170" s="20" t="s">
+        <v>897</v>
+      </c>
+      <c r="I170" s="20" t="s">
         <v>898</v>
-      </c>
-      <c r="H170" s="20" t="s">
-        <v>899</v>
-      </c>
-      <c r="I170" s="20" t="s">
-        <v>900</v>
       </c>
       <c r="J170" s="21" t="s">
         <v>93</v>
@@ -13139,7 +13119,7 @@
         <v>93</v>
       </c>
       <c r="S170" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T170" s="21"/>
       <c r="U170" s="22"/>
@@ -13168,13 +13148,13 @@
         <v>45453</v>
       </c>
       <c r="G171" s="60" t="s">
+        <v>899</v>
+      </c>
+      <c r="H171" s="20" t="s">
+        <v>900</v>
+      </c>
+      <c r="I171" s="20" t="s">
         <v>901</v>
-      </c>
-      <c r="H171" s="20" t="s">
-        <v>902</v>
-      </c>
-      <c r="I171" s="20" t="s">
-        <v>903</v>
       </c>
       <c r="J171" s="21" t="s">
         <v>93</v>
@@ -13198,7 +13178,7 @@
         <v>93</v>
       </c>
       <c r="S171" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T171" s="21"/>
       <c r="U171" s="22"/>
@@ -13227,13 +13207,13 @@
         <v>45453</v>
       </c>
       <c r="G172" s="60" t="s">
+        <v>902</v>
+      </c>
+      <c r="H172" s="20" t="s">
+        <v>903</v>
+      </c>
+      <c r="I172" s="20" t="s">
         <v>904</v>
-      </c>
-      <c r="H172" s="20" t="s">
-        <v>905</v>
-      </c>
-      <c r="I172" s="20" t="s">
-        <v>906</v>
       </c>
       <c r="J172" s="21" t="s">
         <v>93</v>
@@ -13257,7 +13237,7 @@
         <v>93</v>
       </c>
       <c r="S172" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T172" s="21"/>
       <c r="U172" s="22"/>
@@ -13286,13 +13266,13 @@
         <v>45453</v>
       </c>
       <c r="G173" s="60" t="s">
+        <v>905</v>
+      </c>
+      <c r="H173" s="20" t="s">
+        <v>906</v>
+      </c>
+      <c r="I173" s="20" t="s">
         <v>907</v>
-      </c>
-      <c r="H173" s="20" t="s">
-        <v>908</v>
-      </c>
-      <c r="I173" s="20" t="s">
-        <v>909</v>
       </c>
       <c r="J173" s="21" t="s">
         <v>93</v>
@@ -13316,7 +13296,7 @@
         <v>93</v>
       </c>
       <c r="S173" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T173" s="21"/>
       <c r="U173" s="22"/>
@@ -13345,13 +13325,13 @@
         <v>45453</v>
       </c>
       <c r="G174" s="60" t="s">
+        <v>908</v>
+      </c>
+      <c r="H174" s="20" t="s">
+        <v>909</v>
+      </c>
+      <c r="I174" s="20" t="s">
         <v>910</v>
-      </c>
-      <c r="H174" s="20" t="s">
-        <v>911</v>
-      </c>
-      <c r="I174" s="20" t="s">
-        <v>912</v>
       </c>
       <c r="J174" s="21" t="s">
         <v>93</v>
@@ -13375,7 +13355,7 @@
         <v>93</v>
       </c>
       <c r="S174" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T174" s="21"/>
       <c r="U174" s="22"/>
@@ -13404,13 +13384,13 @@
         <v>45453</v>
       </c>
       <c r="G175" s="60" t="s">
+        <v>911</v>
+      </c>
+      <c r="H175" s="20" t="s">
+        <v>912</v>
+      </c>
+      <c r="I175" s="20" t="s">
         <v>913</v>
-      </c>
-      <c r="H175" s="20" t="s">
-        <v>914</v>
-      </c>
-      <c r="I175" s="20" t="s">
-        <v>915</v>
       </c>
       <c r="J175" s="21" t="s">
         <v>93</v>
@@ -13434,7 +13414,7 @@
         <v>93</v>
       </c>
       <c r="S175" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T175" s="21"/>
       <c r="U175" s="22"/>
@@ -13463,13 +13443,13 @@
         <v>45453</v>
       </c>
       <c r="G176" s="60" t="s">
+        <v>914</v>
+      </c>
+      <c r="H176" s="20" t="s">
+        <v>915</v>
+      </c>
+      <c r="I176" s="20" t="s">
         <v>916</v>
-      </c>
-      <c r="H176" s="20" t="s">
-        <v>917</v>
-      </c>
-      <c r="I176" s="20" t="s">
-        <v>918</v>
       </c>
       <c r="J176" s="21" t="s">
         <v>93</v>
@@ -13493,7 +13473,7 @@
         <v>93</v>
       </c>
       <c r="S176" s="21" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="T176" s="21"/>
       <c r="U176" s="22"/>
@@ -20916,19 +20896,19 @@
         <v>726</v>
       </c>
       <c r="E377" s="18" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F377" s="19">
         <v>45453</v>
       </c>
       <c r="G377" s="60" t="s">
+        <v>918</v>
+      </c>
+      <c r="H377" s="20" t="s">
+        <v>919</v>
+      </c>
+      <c r="I377" s="20" t="s">
         <v>920</v>
-      </c>
-      <c r="H377" s="20" t="s">
-        <v>921</v>
-      </c>
-      <c r="I377" s="20" t="s">
-        <v>922</v>
       </c>
       <c r="J377" s="21" t="s">
         <v>93</v>
@@ -21265,7 +21245,7 @@
       <c r="F391" s="12"/>
       <c r="G391" s="12"/>
       <c r="H391" s="12"/>
-      <c r="I391" s="12"/>
+      <c r="I391" s="73"/>
       <c r="J391" s="13"/>
       <c r="K391" s="13"/>
       <c r="L391" s="13"/>
@@ -21285,7 +21265,7 @@
       <c r="F392" s="12"/>
       <c r="G392" s="12"/>
       <c r="H392" s="12"/>
-      <c r="I392" s="12"/>
+      <c r="I392" s="73"/>
       <c r="J392" s="13"/>
       <c r="K392" s="13"/>
       <c r="L392" s="13"/>
@@ -25759,7 +25739,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{F5F4AC7B-142E-4F14-AD0B-95E75DB6B433}">
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
@@ -28570,26 +28550,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf687118-532e-48e1-8af1-d988395d1ed5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100503D4CC5EC91C143B5980EDD06501138" ma:contentTypeVersion="18" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="45bcd79e6cca926293b49fcd4c1ccd23">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf687118-532e-48e1-8af1-d988395d1ed5" xmlns:ns3="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ce83d9c075a3d6749c5f4fbaf20e46d" ns2:_="" ns3:_="">
     <xsd:import namespace="cf687118-532e-48e1-8af1-d988395d1ed5"/>
@@ -28844,10 +28804,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf687118-532e-48e1-8af1-d988395d1ed5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{686AFB90-7606-45ED-AF24-AC61884706CB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cf687118-532e-48e1-8af1-d988395d1ed5"/>
+    <ds:schemaRef ds:uri="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28872,20 +28863,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{686AFB90-7606-45ED-AF24-AC61884706CB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cf687118-532e-48e1-8af1-d988395d1ed5"/>
-    <ds:schemaRef ds:uri="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correzione appId e appVendor in chiamata gtw e ripetizione test
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GASNETGROUPXX/gasnet/SaniPocket/V1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GASNETGROUPXX/gasnet/SaniPocket/V1.0/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE-GTW\GitHubRepo\it-fse-accreditamento\GATEWAY\A1#111#GASNETGROUPXX\gasnet\SaniPocket\V1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simone.bettini\Desktop\temp\SUBMISSION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B94AB5B-B5CD-4224-8047-C8239DE30D31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E021CF-9AA1-4EB6-8F6B-262EA4C83FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -4006,12 +4006,6 @@
     <t>subject_application_version: 1.0</t>
   </si>
   <si>
-    <t>2024-06-10T08:06:39Z</t>
-  </si>
-  <si>
-    <t>6ae8dede4f67d320</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -4025,253 +4019,259 @@
 </t>
   </si>
   <si>
-    <t>2024-06-10T08:07:10Z</t>
-  </si>
-  <si>
-    <t>96a40bac6e5d898f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.0c86db408f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
 </t>
   </si>
   <si>
-    <t>2024-06-10T08:07:17Z</t>
-  </si>
-  <si>
-    <t>7717bd6c358beefd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.c1d7143eda^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
 </t>
   </si>
   <si>
-    <t>2024-06-10T08:07:36Z</t>
-  </si>
-  <si>
-    <t>8e2916c509f645fe</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.017ac6899a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
 </t>
   </si>
   <si>
-    <t>2024-06-10T08:07:49Z</t>
-  </si>
-  <si>
-    <t>ab4f9b928d2f98d9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.7dface1391^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:08:01Z</t>
-  </si>
-  <si>
-    <t>06399a7c5e22f725</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.7cdf82c429^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:08:28Z</t>
-  </si>
-  <si>
-    <t>eacc963553b33e82</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.e84b605f55^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:08:56Z</t>
-  </si>
-  <si>
-    <t>6c6276eb7d62cd29</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.cadc21e25c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:09:11Z</t>
-  </si>
-  <si>
-    <t>a54d586219ddafa5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.587f671c54^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:09:30Z</t>
-  </si>
-  <si>
-    <t>06c7aab7e2425911</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.646fd77b56^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:09:40Z</t>
-  </si>
-  <si>
-    <t>eeb705a81e12834b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.8e07fcc682^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:09:58Z</t>
-  </si>
-  <si>
-    <t>f9aadc4872606a87</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.9ecb980950^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:10:12Z</t>
-  </si>
-  <si>
-    <t>9c34d7c8eb3d2517</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.2fa1f9173c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:10:25Z</t>
-  </si>
-  <si>
-    <t>99de5bc577b25126</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.f7551a8359^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:10:41Z</t>
-  </si>
-  <si>
-    <t>5ed1e455c978929e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.69a884634a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:10:55Z</t>
-  </si>
-  <si>
-    <t>15c3cfd0c23f07a3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.9ef52ad8cd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:11:14Z</t>
-  </si>
-  <si>
-    <t>488cc05110d95150</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.98cdc9d12d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:11:49Z</t>
-  </si>
-  <si>
-    <t>b4d505a3461a0979</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.87e8f55628^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:12:08Z</t>
-  </si>
-  <si>
-    <t>e5b463b8ef1bafd1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.af7d4187a0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:12:55Z</t>
-  </si>
-  <si>
-    <t>dd7d9cb36d5eeb0b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.e7be342d05^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:13:19Z</t>
-  </si>
-  <si>
-    <t>b09f6f8fd04ec31e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.c7d09733d9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:13:43Z</t>
-  </si>
-  <si>
-    <t>2e1c0da75b6531bd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.df59ad1ca7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:14:02Z</t>
-  </si>
-  <si>
-    <t>cef8fe9be0bdd7fd</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.fc819586ec^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2024-06-10T08:14:18Z</t>
-  </si>
-  <si>
-    <t>a000e31b2faa5b29</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.1a3cbf2d78^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation", al fine di una futura pubblicazione, con esito positivo (status code 201), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 Il Documento CDA2 Referto Specialistica Ambulatoriale dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 0" riportata nei documenti "casi di test RSA" e "CDA2_Referto_Specialistica_Ambulatoriale_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.
 </t>
   </si>
   <si>
-    <t>2024-06-10T08:45:46Z</t>
-  </si>
-  <si>
-    <t>71679e944c6415d7</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.657087a48d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Monitoraggio CheckMk - Operatore di Backoffice - Reinvio manuale - Il medico può proseguire a produrre il documento</t>
   </si>
   <si>
-    <t>2024-07-16T07:40:13Z</t>
-  </si>
-  <si>
-    <t>ee6a5105e2b627dd</t>
+    <t>2024-07-17T14:34:58Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:35:16Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:35:32Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:35:44Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:35:51Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:36:00Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:36:06Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:36:23Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:37:00Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:37:05Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:37:11Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:37:18Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:37:23Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:37:29Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:37:37Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:37:42Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:37:49Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:37:55Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:38:01Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:38:10Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:38:20Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:38:26Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:38:32Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:38:38Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:38:51Z</t>
+  </si>
+  <si>
+    <t>2024-07-17T14:38:58Z</t>
+  </si>
+  <si>
+    <t>9d91b9d1c6554d14</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>525700fdcaba9d59</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.1fbadafeaf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>06fccd41e3da71c3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.37e75c39e3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>c7c275fc2ab244d1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.703368d31b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>52c466e99beb603d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.3bed5a85ae^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>bb7ac3c154dc8bd6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.2cdd25eb7e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>d4f93bc8decac491</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.a7b8e68fcc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>fa8ee9d88a194640</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.588975a5e3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>9f0a514e83f11974</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.1ecc48e19f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>947026aec73385bc</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.ea0130313a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4ebde6adc9e704af</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.add531cf99^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>45030b8d5a6fff6c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.58dba61cf6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>fa058c48326affec</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.96087ee1ab^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>e6efd6c7ee3c31f0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.35b394daf4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ac5ffc0d79015204</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.dc6c0ea037^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4b5aaee14addbe01</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.92b6fadbda^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f94fa0d191863ac9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.1ee019fea7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f1d077aeec938f30</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.0c7416d0b2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5e7d6bf7fccc5c3d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.ae9af6e36f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>a608df235dd2b759</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.073bf1ab72^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>0033bf17c34f4b6f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.cc48f6e06d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>d5cefca35eb2ed94</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.9b6194a89b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>0cc7d8dcc5dd9809</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.feb182bc8b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>af160d1748659f02</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.b683468b6f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>584502cd83a8959c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.df38d7e172^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4980,6 +4980,9 @@
     <xf numFmtId="22" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5001,9 +5004,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6486,7 +6486,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I392" sqref="I391:I392"/>
+      <selection pane="bottomRight" activeCell="I394" sqref="I394"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6528,12 +6528,12 @@
       <c r="W1" s="15"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="65"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -6554,14 +6554,14 @@
       <c r="W2" s="15"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="72" t="s">
+      <c r="B3" s="68"/>
+      <c r="C3" s="73" t="s">
         <v>837</v>
       </c>
-      <c r="D3" s="64"/>
+      <c r="D3" s="65"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -6582,12 +6582,12 @@
       <c r="W3" s="15"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68"/>
-      <c r="B4" s="69"/>
-      <c r="C4" s="72" t="s">
+      <c r="A4" s="69"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="73" t="s">
         <v>838</v>
       </c>
-      <c r="D4" s="64"/>
+      <c r="D4" s="65"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -6609,12 +6609,12 @@
       <c r="W4" s="15"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="72" t="s">
+      <c r="A5" s="71"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="73" t="s">
         <v>839</v>
       </c>
-      <c r="D5" s="64"/>
+      <c r="D5" s="65"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -6635,8 +6635,8 @@
       <c r="W5" s="15"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="61"/>
-      <c r="B6" s="62"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="63"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -7861,16 +7861,16 @@
         <v>72</v>
       </c>
       <c r="F39" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G39" s="60" t="s">
+        <v>848</v>
+      </c>
+      <c r="H39" s="20" t="s">
+        <v>874</v>
+      </c>
+      <c r="I39" s="20" t="s">
         <v>840</v>
-      </c>
-      <c r="H39" s="20" t="s">
-        <v>841</v>
-      </c>
-      <c r="I39" s="20" t="s">
-        <v>842</v>
       </c>
       <c r="J39" s="21" t="s">
         <v>93</v>
@@ -7894,7 +7894,7 @@
         <v>93</v>
       </c>
       <c r="S39" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T39" s="21"/>
       <c r="U39" s="21"/>
@@ -8179,16 +8179,16 @@
         <v>84</v>
       </c>
       <c r="F47" s="19">
-        <v>45489</v>
+        <v>45490</v>
       </c>
       <c r="G47" s="60" t="s">
-        <v>922</v>
+        <v>849</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>923</v>
+        <v>875</v>
       </c>
       <c r="I47" s="20" t="s">
-        <v>842</v>
+        <v>875</v>
       </c>
       <c r="J47" s="21" t="s">
         <v>93</v>
@@ -8212,7 +8212,7 @@
         <v>93</v>
       </c>
       <c r="S47" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T47" s="21"/>
       <c r="U47" s="21"/>
@@ -8502,7 +8502,7 @@
         <v>97</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="F55" s="19"/>
       <c r="G55" s="60"/>
@@ -8530,7 +8530,7 @@
         <v>93</v>
       </c>
       <c r="S55" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T55" s="21"/>
       <c r="U55" s="22" t="s">
@@ -12187,19 +12187,19 @@
         <v>291</v>
       </c>
       <c r="E154" s="18" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="F154" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G154" s="60" t="s">
-        <v>845</v>
+        <v>850</v>
       </c>
       <c r="H154" s="20" t="s">
-        <v>846</v>
+        <v>876</v>
       </c>
       <c r="I154" s="20" t="s">
-        <v>847</v>
+        <v>877</v>
       </c>
       <c r="J154" s="21" t="s">
         <v>93</v>
@@ -12234,19 +12234,19 @@
         <v>292</v>
       </c>
       <c r="E155" s="18" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="F155" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G155" s="60" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="H155" s="20" t="s">
-        <v>850</v>
+        <v>878</v>
       </c>
       <c r="I155" s="20" t="s">
-        <v>851</v>
+        <v>879</v>
       </c>
       <c r="J155" s="21" t="s">
         <v>93</v>
@@ -12281,19 +12281,19 @@
         <v>293</v>
       </c>
       <c r="E156" s="18" t="s">
+        <v>844</v>
+      </c>
+      <c r="F156" s="19">
+        <v>45490</v>
+      </c>
+      <c r="G156" s="60" t="s">
         <v>852</v>
       </c>
-      <c r="F156" s="19">
-        <v>45453</v>
-      </c>
-      <c r="G156" s="60" t="s">
-        <v>853</v>
-      </c>
       <c r="H156" s="20" t="s">
-        <v>854</v>
+        <v>880</v>
       </c>
       <c r="I156" s="20" t="s">
-        <v>855</v>
+        <v>881</v>
       </c>
       <c r="J156" s="21" t="s">
         <v>93</v>
@@ -12328,19 +12328,19 @@
         <v>294</v>
       </c>
       <c r="E157" s="18" t="s">
-        <v>856</v>
+        <v>845</v>
       </c>
       <c r="F157" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G157" s="60" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="H157" s="20" t="s">
-        <v>858</v>
+        <v>882</v>
       </c>
       <c r="I157" s="20" t="s">
-        <v>859</v>
+        <v>883</v>
       </c>
       <c r="J157" s="21" t="s">
         <v>93</v>
@@ -12378,16 +12378,16 @@
         <v>296</v>
       </c>
       <c r="F158" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G158" s="60" t="s">
-        <v>860</v>
+        <v>854</v>
       </c>
       <c r="H158" s="20" t="s">
-        <v>861</v>
+        <v>884</v>
       </c>
       <c r="I158" s="20" t="s">
-        <v>862</v>
+        <v>885</v>
       </c>
       <c r="J158" s="21" t="s">
         <v>93</v>
@@ -12411,7 +12411,7 @@
         <v>93</v>
       </c>
       <c r="S158" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T158" s="21"/>
       <c r="U158" s="22"/>
@@ -12437,16 +12437,16 @@
         <v>298</v>
       </c>
       <c r="F159" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G159" s="60" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="H159" s="20" t="s">
-        <v>864</v>
+        <v>886</v>
       </c>
       <c r="I159" s="20" t="s">
-        <v>865</v>
+        <v>887</v>
       </c>
       <c r="J159" s="21" t="s">
         <v>93</v>
@@ -12470,7 +12470,7 @@
         <v>93</v>
       </c>
       <c r="S159" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T159" s="21"/>
       <c r="U159" s="22"/>
@@ -12496,16 +12496,16 @@
         <v>300</v>
       </c>
       <c r="F160" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G160" s="60" t="s">
-        <v>866</v>
+        <v>856</v>
       </c>
       <c r="H160" s="20" t="s">
-        <v>867</v>
+        <v>888</v>
       </c>
       <c r="I160" s="20" t="s">
-        <v>868</v>
+        <v>889</v>
       </c>
       <c r="J160" s="21" t="s">
         <v>93</v>
@@ -12529,7 +12529,7 @@
         <v>93</v>
       </c>
       <c r="S160" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T160" s="21"/>
       <c r="U160" s="22"/>
@@ -12555,16 +12555,16 @@
         <v>302</v>
       </c>
       <c r="F161" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G161" s="60" t="s">
-        <v>869</v>
+        <v>857</v>
       </c>
       <c r="H161" s="20" t="s">
-        <v>870</v>
+        <v>890</v>
       </c>
       <c r="I161" s="20" t="s">
-        <v>871</v>
+        <v>891</v>
       </c>
       <c r="J161" s="21" t="s">
         <v>93</v>
@@ -12588,7 +12588,7 @@
         <v>93</v>
       </c>
       <c r="S161" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T161" s="21"/>
       <c r="U161" s="22"/>
@@ -12614,16 +12614,16 @@
         <v>304</v>
       </c>
       <c r="F162" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G162" s="60" t="s">
-        <v>872</v>
+        <v>858</v>
       </c>
       <c r="H162" s="20" t="s">
-        <v>873</v>
+        <v>892</v>
       </c>
       <c r="I162" s="20" t="s">
-        <v>874</v>
+        <v>893</v>
       </c>
       <c r="J162" s="21" t="s">
         <v>93</v>
@@ -12647,7 +12647,7 @@
         <v>93</v>
       </c>
       <c r="S162" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T162" s="21"/>
       <c r="U162" s="22"/>
@@ -12673,16 +12673,16 @@
         <v>306</v>
       </c>
       <c r="F163" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G163" s="60" t="s">
-        <v>875</v>
+        <v>859</v>
       </c>
       <c r="H163" s="20" t="s">
-        <v>876</v>
+        <v>894</v>
       </c>
       <c r="I163" s="20" t="s">
-        <v>877</v>
+        <v>895</v>
       </c>
       <c r="J163" s="21" t="s">
         <v>93</v>
@@ -12706,7 +12706,7 @@
         <v>93</v>
       </c>
       <c r="S163" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T163" s="21"/>
       <c r="U163" s="22"/>
@@ -12732,16 +12732,16 @@
         <v>308</v>
       </c>
       <c r="F164" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G164" s="60" t="s">
-        <v>878</v>
+        <v>860</v>
       </c>
       <c r="H164" s="20" t="s">
-        <v>879</v>
+        <v>896</v>
       </c>
       <c r="I164" s="20" t="s">
-        <v>880</v>
+        <v>897</v>
       </c>
       <c r="J164" s="21" t="s">
         <v>93</v>
@@ -12765,7 +12765,7 @@
         <v>93</v>
       </c>
       <c r="S164" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T164" s="21"/>
       <c r="U164" s="22"/>
@@ -12791,16 +12791,16 @@
         <v>310</v>
       </c>
       <c r="F165" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G165" s="60" t="s">
-        <v>881</v>
+        <v>861</v>
       </c>
       <c r="H165" s="20" t="s">
-        <v>882</v>
+        <v>898</v>
       </c>
       <c r="I165" s="20" t="s">
-        <v>883</v>
+        <v>899</v>
       </c>
       <c r="J165" s="21" t="s">
         <v>93</v>
@@ -12824,7 +12824,7 @@
         <v>93</v>
       </c>
       <c r="S165" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T165" s="21"/>
       <c r="U165" s="22"/>
@@ -12850,16 +12850,16 @@
         <v>312</v>
       </c>
       <c r="F166" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G166" s="60" t="s">
-        <v>884</v>
+        <v>862</v>
       </c>
       <c r="H166" s="20" t="s">
-        <v>885</v>
+        <v>900</v>
       </c>
       <c r="I166" s="20" t="s">
-        <v>886</v>
+        <v>901</v>
       </c>
       <c r="J166" s="21" t="s">
         <v>93</v>
@@ -12883,7 +12883,7 @@
         <v>93</v>
       </c>
       <c r="S166" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T166" s="21"/>
       <c r="U166" s="22"/>
@@ -12909,16 +12909,16 @@
         <v>314</v>
       </c>
       <c r="F167" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G167" s="60" t="s">
-        <v>887</v>
+        <v>863</v>
       </c>
       <c r="H167" s="20" t="s">
-        <v>888</v>
+        <v>902</v>
       </c>
       <c r="I167" s="20" t="s">
-        <v>889</v>
+        <v>903</v>
       </c>
       <c r="J167" s="21" t="s">
         <v>93</v>
@@ -12942,7 +12942,7 @@
         <v>93</v>
       </c>
       <c r="S167" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T167" s="21"/>
       <c r="U167" s="22"/>
@@ -12968,16 +12968,16 @@
         <v>316</v>
       </c>
       <c r="F168" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G168" s="60" t="s">
-        <v>890</v>
+        <v>864</v>
       </c>
       <c r="H168" s="20" t="s">
-        <v>891</v>
+        <v>904</v>
       </c>
       <c r="I168" s="20" t="s">
-        <v>892</v>
+        <v>905</v>
       </c>
       <c r="J168" s="21" t="s">
         <v>93</v>
@@ -13001,7 +13001,7 @@
         <v>93</v>
       </c>
       <c r="S168" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T168" s="21"/>
       <c r="U168" s="22"/>
@@ -13027,16 +13027,16 @@
         <v>318</v>
       </c>
       <c r="F169" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G169" s="60" t="s">
-        <v>893</v>
+        <v>865</v>
       </c>
       <c r="H169" s="20" t="s">
-        <v>894</v>
+        <v>906</v>
       </c>
       <c r="I169" s="20" t="s">
-        <v>895</v>
+        <v>907</v>
       </c>
       <c r="J169" s="21" t="s">
         <v>93</v>
@@ -13060,7 +13060,7 @@
         <v>93</v>
       </c>
       <c r="S169" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T169" s="21"/>
       <c r="U169" s="22"/>
@@ -13086,16 +13086,16 @@
         <v>320</v>
       </c>
       <c r="F170" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G170" s="60" t="s">
-        <v>896</v>
+        <v>866</v>
       </c>
       <c r="H170" s="20" t="s">
-        <v>897</v>
+        <v>908</v>
       </c>
       <c r="I170" s="20" t="s">
-        <v>898</v>
+        <v>909</v>
       </c>
       <c r="J170" s="21" t="s">
         <v>93</v>
@@ -13119,7 +13119,7 @@
         <v>93</v>
       </c>
       <c r="S170" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T170" s="21"/>
       <c r="U170" s="22"/>
@@ -13145,16 +13145,16 @@
         <v>322</v>
       </c>
       <c r="F171" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G171" s="60" t="s">
-        <v>899</v>
+        <v>867</v>
       </c>
       <c r="H171" s="20" t="s">
-        <v>900</v>
+        <v>910</v>
       </c>
       <c r="I171" s="20" t="s">
-        <v>901</v>
+        <v>911</v>
       </c>
       <c r="J171" s="21" t="s">
         <v>93</v>
@@ -13178,7 +13178,7 @@
         <v>93</v>
       </c>
       <c r="S171" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T171" s="21"/>
       <c r="U171" s="22"/>
@@ -13204,16 +13204,16 @@
         <v>324</v>
       </c>
       <c r="F172" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G172" s="60" t="s">
-        <v>902</v>
+        <v>868</v>
       </c>
       <c r="H172" s="20" t="s">
-        <v>903</v>
+        <v>912</v>
       </c>
       <c r="I172" s="20" t="s">
-        <v>904</v>
+        <v>913</v>
       </c>
       <c r="J172" s="21" t="s">
         <v>93</v>
@@ -13237,7 +13237,7 @@
         <v>93</v>
       </c>
       <c r="S172" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T172" s="21"/>
       <c r="U172" s="22"/>
@@ -13263,16 +13263,16 @@
         <v>326</v>
       </c>
       <c r="F173" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G173" s="60" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="H173" s="20" t="s">
-        <v>906</v>
+        <v>914</v>
       </c>
       <c r="I173" s="20" t="s">
-        <v>907</v>
+        <v>915</v>
       </c>
       <c r="J173" s="21" t="s">
         <v>93</v>
@@ -13296,7 +13296,7 @@
         <v>93</v>
       </c>
       <c r="S173" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T173" s="21"/>
       <c r="U173" s="22"/>
@@ -13322,16 +13322,16 @@
         <v>328</v>
       </c>
       <c r="F174" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G174" s="60" t="s">
-        <v>908</v>
+        <v>870</v>
       </c>
       <c r="H174" s="20" t="s">
-        <v>909</v>
+        <v>916</v>
       </c>
       <c r="I174" s="20" t="s">
-        <v>910</v>
+        <v>917</v>
       </c>
       <c r="J174" s="21" t="s">
         <v>93</v>
@@ -13355,7 +13355,7 @@
         <v>93</v>
       </c>
       <c r="S174" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T174" s="21"/>
       <c r="U174" s="22"/>
@@ -13381,16 +13381,16 @@
         <v>330</v>
       </c>
       <c r="F175" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G175" s="60" t="s">
-        <v>911</v>
+        <v>871</v>
       </c>
       <c r="H175" s="20" t="s">
-        <v>912</v>
+        <v>918</v>
       </c>
       <c r="I175" s="20" t="s">
-        <v>913</v>
+        <v>919</v>
       </c>
       <c r="J175" s="21" t="s">
         <v>93</v>
@@ -13414,7 +13414,7 @@
         <v>93</v>
       </c>
       <c r="S175" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T175" s="21"/>
       <c r="U175" s="22"/>
@@ -13440,16 +13440,16 @@
         <v>332</v>
       </c>
       <c r="F176" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G176" s="60" t="s">
-        <v>914</v>
+        <v>872</v>
       </c>
       <c r="H176" s="20" t="s">
-        <v>915</v>
+        <v>920</v>
       </c>
       <c r="I176" s="20" t="s">
-        <v>916</v>
+        <v>921</v>
       </c>
       <c r="J176" s="21" t="s">
         <v>93</v>
@@ -13473,7 +13473,7 @@
         <v>93</v>
       </c>
       <c r="S176" s="21" t="s">
-        <v>921</v>
+        <v>847</v>
       </c>
       <c r="T176" s="21"/>
       <c r="U176" s="22"/>
@@ -20896,19 +20896,19 @@
         <v>726</v>
       </c>
       <c r="E377" s="18" t="s">
-        <v>917</v>
+        <v>846</v>
       </c>
       <c r="F377" s="19">
-        <v>45453</v>
+        <v>45490</v>
       </c>
       <c r="G377" s="60" t="s">
-        <v>918</v>
+        <v>873</v>
       </c>
       <c r="H377" s="20" t="s">
-        <v>919</v>
+        <v>922</v>
       </c>
       <c r="I377" s="20" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="J377" s="21" t="s">
         <v>93</v>
@@ -21245,7 +21245,7 @@
       <c r="F391" s="12"/>
       <c r="G391" s="12"/>
       <c r="H391" s="12"/>
-      <c r="I391" s="73"/>
+      <c r="I391" s="61"/>
       <c r="J391" s="13"/>
       <c r="K391" s="13"/>
       <c r="L391" s="13"/>
@@ -21265,7 +21265,7 @@
       <c r="F392" s="12"/>
       <c r="G392" s="12"/>
       <c r="H392" s="12"/>
-      <c r="I392" s="73"/>
+      <c r="I392" s="61"/>
       <c r="J392" s="13"/>
       <c r="K392" s="13"/>
       <c r="L392" s="13"/>
@@ -28550,6 +28550,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf687118-532e-48e1-8af1-d988395d1ed5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100503D4CC5EC91C143B5980EDD06501138" ma:contentTypeVersion="18" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="45bcd79e6cca926293b49fcd4c1ccd23">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf687118-532e-48e1-8af1-d988395d1ed5" xmlns:ns3="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ce83d9c075a3d6749c5f4fbaf20e46d" ns2:_="" ns3:_="">
     <xsd:import namespace="cf687118-532e-48e1-8af1-d988395d1ed5"/>
@@ -28804,41 +28824,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf687118-532e-48e1-8af1-d988395d1ed5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{686AFB90-7606-45ED-AF24-AC61884706CB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cf687118-532e-48e1-8af1-d988395d1ed5"/>
-    <ds:schemaRef ds:uri="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28863,9 +28852,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{686AFB90-7606-45ED-AF24-AC61884706CB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cf687118-532e-48e1-8af1-d988395d1ed5"/>
+    <ds:schemaRef ds:uri="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Correzione test case 40
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#GASNETGROUPXX/gasnet/SaniPocket/V1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111#GASNETGROUPXX/gasnet/SaniPocket/V1.0/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simone.bettini\Desktop\temp\SUBMISSION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE-GTW\GitHubRepo\it-fse-accreditamento\GATEWAY\A1#111#GASNETGROUPXX\gasnet\SaniPocket\V1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E021CF-9AA1-4EB6-8F6B-262EA4C83FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFD2186-DED2-4EA2-AEAC-2ED5FF8DB36F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4049,9 +4049,6 @@
     <t>2024-07-17T14:34:58Z</t>
   </si>
   <si>
-    <t>2024-07-17T14:35:16Z</t>
-  </si>
-  <si>
     <t>2024-07-17T14:35:32Z</t>
   </si>
   <si>
@@ -4127,9 +4124,6 @@
     <t>9d91b9d1c6554d14</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>525700fdcaba9d59</t>
   </si>
   <si>
@@ -4272,6 +4266,12 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.2149fb78666c205ac20b9bd2d882af037f0819429c691196eaa8054488c56c20.df38d7e172^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2024-07-18T07:33:25Z</t>
+  </si>
+  <si>
+    <t>42828fa3b91aac93</t>
   </si>
 </sst>
 </file>
@@ -6483,10 +6483,10 @@
   <dimension ref="A1:W968"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I394" sqref="I394"/>
+      <selection pane="bottomRight" activeCell="J393" sqref="J393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7867,7 +7867,7 @@
         <v>848</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="I39" s="20" t="s">
         <v>840</v>
@@ -8179,16 +8179,16 @@
         <v>84</v>
       </c>
       <c r="F47" s="19">
-        <v>45490</v>
+        <v>45491</v>
       </c>
       <c r="G47" s="60" t="s">
-        <v>849</v>
+        <v>922</v>
       </c>
       <c r="H47" s="20" t="s">
-        <v>875</v>
+        <v>923</v>
       </c>
       <c r="I47" s="20" t="s">
-        <v>875</v>
+        <v>840</v>
       </c>
       <c r="J47" s="21" t="s">
         <v>93</v>
@@ -12193,13 +12193,13 @@
         <v>45490</v>
       </c>
       <c r="G154" s="60" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="H154" s="20" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="I154" s="20" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="J154" s="21" t="s">
         <v>93</v>
@@ -12240,13 +12240,13 @@
         <v>45490</v>
       </c>
       <c r="G155" s="60" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="H155" s="20" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="I155" s="20" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="J155" s="21" t="s">
         <v>93</v>
@@ -12287,13 +12287,13 @@
         <v>45490</v>
       </c>
       <c r="G156" s="60" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="H156" s="20" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="I156" s="20" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="J156" s="21" t="s">
         <v>93</v>
@@ -12334,13 +12334,13 @@
         <v>45490</v>
       </c>
       <c r="G157" s="60" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="H157" s="20" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="I157" s="20" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="J157" s="21" t="s">
         <v>93</v>
@@ -12381,13 +12381,13 @@
         <v>45490</v>
       </c>
       <c r="G158" s="60" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="H158" s="20" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="I158" s="20" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="J158" s="21" t="s">
         <v>93</v>
@@ -12440,13 +12440,13 @@
         <v>45490</v>
       </c>
       <c r="G159" s="60" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H159" s="20" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="I159" s="20" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="J159" s="21" t="s">
         <v>93</v>
@@ -12499,13 +12499,13 @@
         <v>45490</v>
       </c>
       <c r="G160" s="60" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="H160" s="20" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="I160" s="20" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="J160" s="21" t="s">
         <v>93</v>
@@ -12558,13 +12558,13 @@
         <v>45490</v>
       </c>
       <c r="G161" s="60" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="H161" s="20" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="I161" s="20" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="J161" s="21" t="s">
         <v>93</v>
@@ -12617,13 +12617,13 @@
         <v>45490</v>
       </c>
       <c r="G162" s="60" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="H162" s="20" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="I162" s="20" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="J162" s="21" t="s">
         <v>93</v>
@@ -12676,13 +12676,13 @@
         <v>45490</v>
       </c>
       <c r="G163" s="60" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="H163" s="20" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="I163" s="20" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="J163" s="21" t="s">
         <v>93</v>
@@ -12735,13 +12735,13 @@
         <v>45490</v>
       </c>
       <c r="G164" s="60" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="H164" s="20" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="I164" s="20" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="J164" s="21" t="s">
         <v>93</v>
@@ -12794,13 +12794,13 @@
         <v>45490</v>
       </c>
       <c r="G165" s="60" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="H165" s="20" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="I165" s="20" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="J165" s="21" t="s">
         <v>93</v>
@@ -12853,13 +12853,13 @@
         <v>45490</v>
       </c>
       <c r="G166" s="60" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="H166" s="20" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="I166" s="20" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="J166" s="21" t="s">
         <v>93</v>
@@ -12912,13 +12912,13 @@
         <v>45490</v>
       </c>
       <c r="G167" s="60" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="H167" s="20" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="I167" s="20" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="J167" s="21" t="s">
         <v>93</v>
@@ -12971,13 +12971,13 @@
         <v>45490</v>
       </c>
       <c r="G168" s="60" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="H168" s="20" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="I168" s="20" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="J168" s="21" t="s">
         <v>93</v>
@@ -13030,13 +13030,13 @@
         <v>45490</v>
       </c>
       <c r="G169" s="60" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="H169" s="20" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="I169" s="20" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="J169" s="21" t="s">
         <v>93</v>
@@ -13089,13 +13089,13 @@
         <v>45490</v>
       </c>
       <c r="G170" s="60" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="H170" s="20" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="I170" s="20" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="J170" s="21" t="s">
         <v>93</v>
@@ -13148,13 +13148,13 @@
         <v>45490</v>
       </c>
       <c r="G171" s="60" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="H171" s="20" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="I171" s="20" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="J171" s="21" t="s">
         <v>93</v>
@@ -13207,13 +13207,13 @@
         <v>45490</v>
       </c>
       <c r="G172" s="60" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H172" s="20" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="I172" s="20" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="J172" s="21" t="s">
         <v>93</v>
@@ -13266,13 +13266,13 @@
         <v>45490</v>
       </c>
       <c r="G173" s="60" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="H173" s="20" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="I173" s="20" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="J173" s="21" t="s">
         <v>93</v>
@@ -13325,13 +13325,13 @@
         <v>45490</v>
       </c>
       <c r="G174" s="60" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="H174" s="20" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="I174" s="20" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="J174" s="21" t="s">
         <v>93</v>
@@ -13384,13 +13384,13 @@
         <v>45490</v>
       </c>
       <c r="G175" s="60" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="H175" s="20" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="I175" s="20" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="J175" s="21" t="s">
         <v>93</v>
@@ -13443,13 +13443,13 @@
         <v>45490</v>
       </c>
       <c r="G176" s="60" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="H176" s="20" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="I176" s="20" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="J176" s="21" t="s">
         <v>93</v>
@@ -20902,13 +20902,13 @@
         <v>45490</v>
       </c>
       <c r="G377" s="60" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H377" s="20" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="I377" s="20" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="J377" s="21" t="s">
         <v>93</v>
@@ -28550,26 +28550,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf687118-532e-48e1-8af1-d988395d1ed5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100503D4CC5EC91C143B5980EDD06501138" ma:contentTypeVersion="18" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="45bcd79e6cca926293b49fcd4c1ccd23">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cf687118-532e-48e1-8af1-d988395d1ed5" xmlns:ns3="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0ce83d9c075a3d6749c5f4fbaf20e46d" ns2:_="" ns3:_="">
     <xsd:import namespace="cf687118-532e-48e1-8af1-d988395d1ed5"/>
@@ -28824,10 +28804,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cf687118-532e-48e1-8af1-d988395d1ed5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{686AFB90-7606-45ED-AF24-AC61884706CB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cf687118-532e-48e1-8af1-d988395d1ed5"/>
+    <ds:schemaRef ds:uri="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28852,20 +28863,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{686AFB90-7606-45ED-AF24-AC61884706CB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cf687118-532e-48e1-8af1-d988395d1ed5"/>
-    <ds:schemaRef ds:uri="d4f1cf6c-7afe-4da6-9808-35ef0f55ffc6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>